<commit_message>
updated changes for copy columns with multiple sheets
</commit_message>
<xml_diff>
--- a/sample_final.xlsx
+++ b/sample_final.xlsx
@@ -32,7 +32,6 @@
     <definedName name="tdc">'Asset Codes'!$A$24</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2475,6 +2474,51 @@
     <xf numFmtId="177" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2493,51 +2537,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2801,10 +2800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AF115"/>
+  <dimension ref="A2:AF133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.375" defaultRowHeight="18.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2847,7 +2846,7 @@
     <col min="48" max="16384" width="7.375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" ht="18.75" customHeight="1">
+    <row r="2" spans="1:27" ht="18.75" customHeight="1">
       <c r="A2" s="4"/>
       <c r="C2" s="5"/>
       <c r="E2" s="6">
@@ -2894,14 +2893,8 @@
       <c r="AA2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:27" ht="18.75" customHeight="1">
       <c r="A3" s="4"/>
       <c r="C3" s="13"/>
       <c r="D3" s="14"/>
@@ -2936,15 +2929,8 @@
         <v>8</v>
       </c>
       <c r="AA3" s="17"/>
-      <c r="AD3" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" s="18">
-        <f>N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:27" ht="18.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="C4" s="19"/>
       <c r="D4" s="20"/>
@@ -2975,17 +2961,8 @@
       <c r="Y4" s="21"/>
       <c r="Z4" s="22"/>
       <c r="AA4" s="23"/>
-      <c r="AD4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF4" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:27" ht="18.75" customHeight="1">
       <c r="A5" s="4"/>
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
@@ -3012,17 +2989,8 @@
       <c r="Y5" s="24"/>
       <c r="Z5" s="26"/>
       <c r="AA5" s="27"/>
-      <c r="AD5" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE5" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF5" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:27" ht="18.75" customHeight="1">
       <c r="A6" s="28">
         <v>100</v>
       </c>
@@ -3063,17 +3031,8 @@
         <v>0</v>
       </c>
       <c r="AA6" s="27"/>
-      <c r="AD6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF6" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:27" ht="18.75" customHeight="1">
       <c r="A7" s="28"/>
       <c r="C7" s="29" t="s">
         <v>10</v>
@@ -3112,11 +3071,8 @@
         <v>0</v>
       </c>
       <c r="AA7" s="27"/>
-      <c r="AD7" s="12"/>
-      <c r="AE7" s="12"/>
-      <c r="AF7" s="12"/>
-    </row>
-    <row r="8" spans="1:32" ht="18.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:27" ht="18.75" customHeight="1">
       <c r="A8" s="28"/>
       <c r="C8" s="29"/>
       <c r="D8" s="25"/>
@@ -3143,11 +3099,8 @@
       <c r="Y8" s="24"/>
       <c r="Z8" s="30"/>
       <c r="AA8" s="27"/>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-    </row>
-    <row r="9" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    </row>
+    <row r="9" spans="1:27" ht="18.75" customHeight="1">
       <c r="A9" s="28"/>
       <c r="C9" s="29" t="s">
         <v>30</v>
@@ -3176,20 +3129,8 @@
       <c r="Y9" s="24"/>
       <c r="Z9" s="30"/>
       <c r="AA9" s="27"/>
-      <c r="AD9" s="12" t="str">
-        <f>"'"&amp;$AD3&amp;"'"&amp;"!"&amp;AD5</f>
-        <v>'Asset Codes'!$H$1:$BZ$1</v>
-      </c>
-      <c r="AE9" s="12" t="str">
-        <f>"'"&amp;$AD3&amp;"'"&amp;"!"&amp;AE5</f>
-        <v>'Asset Codes'!$B$2:$B$500</v>
-      </c>
-      <c r="AF9" s="12" t="str">
-        <f>"'"&amp;$AD3&amp;"'"&amp;"!"&amp;AF5</f>
-        <v>'Asset Codes'!$H$2:$BZ$500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    </row>
+    <row r="10" spans="1:27" ht="18.75" customHeight="1">
       <c r="A10" s="28"/>
       <c r="C10" s="29"/>
       <c r="D10" s="25"/>
@@ -3216,11 +3157,8 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="30"/>
       <c r="AA10" s="27"/>
-      <c r="AD10" s="32"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="32"/>
-    </row>
-    <row r="11" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    </row>
+    <row r="11" spans="1:27" ht="18.75" customHeight="1">
       <c r="A11" s="4"/>
       <c r="C11" s="29" t="s">
         <v>31</v>
@@ -3250,7 +3188,7 @@
       <c r="Z11" s="30"/>
       <c r="AA11" s="27"/>
     </row>
-    <row r="12" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:27" ht="18.75" customHeight="1">
       <c r="A12" s="4"/>
       <c r="C12" s="29" t="s">
         <v>32</v>
@@ -3280,7 +3218,7 @@
       <c r="Z12" s="30"/>
       <c r="AA12" s="27"/>
     </row>
-    <row r="13" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:27" ht="18.75" customHeight="1">
       <c r="A13" s="4"/>
       <c r="C13" s="29"/>
       <c r="D13" s="25"/>
@@ -3308,7 +3246,7 @@
       <c r="Z13" s="30"/>
       <c r="AA13" s="27"/>
     </row>
-    <row r="14" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:27" ht="18.75" customHeight="1">
       <c r="A14" s="4"/>
       <c r="C14" s="29" t="s">
         <v>33</v>
@@ -3338,7 +3276,7 @@
       <c r="Z14" s="30"/>
       <c r="AA14" s="27"/>
     </row>
-    <row r="15" spans="1:32" ht="18.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:27" ht="18.75" customHeight="1">
       <c r="A15" s="4"/>
       <c r="C15" s="29" t="s">
         <v>34</v>
@@ -3368,7 +3306,7 @@
       <c r="Z15" s="30"/>
       <c r="AA15" s="27"/>
     </row>
-    <row r="16" spans="1:32" ht="18.75" customHeight="1">
+    <row r="16" spans="1:27" ht="18.75" customHeight="1">
       <c r="A16" s="4"/>
       <c r="C16" s="33"/>
       <c r="D16" s="34"/>
@@ -3511,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="54">
-        <f>IFERROR(I19/I$32,0)</f>
+        <f ca="1">IFERROR(I19/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L19" s="25"/>
@@ -3577,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="62">
-        <f>IFERROR(I20/I$32,0)</f>
+        <f ca="1">IFERROR(I20/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L20" s="25"/>
@@ -3695,15 +3633,15 @@
       </c>
       <c r="H23" s="25"/>
       <c r="I23" s="52">
-        <f t="array" ref="I23">IFERROR(SUM(IF($A23=INDIRECT($AE$9),IF(I$2&lt;=INDIRECT($AD$9),IF(J$2&gt;=INDIRECT($AD$9),INDIRECT($AF$9)/I$94,""),""),"")),0)</f>
-        <v>3.27868852459016</v>
+        <f t="array" aca="1" ref="I23" ca="1">IFERROR(SUM(IF($A23=INDIRECT($B$131),IF(I$2&lt;=INDIRECT($A$131),IF(J$2&gt;=INDIRECT($A$131),INDIRECT($C$131)/I$94,""),""),"")),0)</f>
+        <v>3.2786885245901636</v>
       </c>
       <c r="J23" s="53">
-        <f>J47</f>
-        <v>56103.849888888901</v>
+        <f ca="1">J47</f>
+        <v>56103.849888888908</v>
       </c>
       <c r="K23" s="54">
-        <f>IFERROR(I23/I$32,0)</f>
+        <f ca="1">IFERROR(I23/I$32,0)</f>
         <v>1</v>
       </c>
       <c r="L23" s="25"/>
@@ -3774,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="54">
-        <f>IFERROR(I24/I$32,0)</f>
+        <f ca="1">IFERROR(I24/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L24" s="25"/>
@@ -3835,15 +3773,15 @@
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="60">
-        <f>SUM(I23:I24)</f>
-        <v>3.27868852459016</v>
+        <f ca="1">SUM(I23:I24)</f>
+        <v>3.2786885245901636</v>
       </c>
       <c r="J25" s="61">
-        <f>J49</f>
-        <v>56103.849888888901</v>
+        <f ca="1">J49</f>
+        <v>56103.849888888908</v>
       </c>
       <c r="K25" s="62">
-        <f>IFERROR(I25/I$32,0)</f>
+        <f ca="1">IFERROR(I25/I$32,0)</f>
         <v>1</v>
       </c>
       <c r="L25" s="25"/>
@@ -3978,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="54">
-        <f>IFERROR(I28/I$32,0)</f>
+        <f ca="1">IFERROR(I28/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L28" s="25"/>
@@ -4049,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="54">
-        <f>IFERROR(I29/I$32,0)</f>
+        <f ca="1">IFERROR(I29/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L29" s="25"/>
@@ -4118,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="62">
-        <f>IFERROR(I30/I$32,0)</f>
+        <f ca="1">IFERROR(I30/I$32,0)</f>
         <v>0</v>
       </c>
       <c r="L30" s="25"/>
@@ -4210,15 +4148,15 @@
       </c>
       <c r="H32" s="25"/>
       <c r="I32" s="60">
-        <f>I20+I25+I30</f>
-        <v>3.27868852459016</v>
+        <f ca="1">I20+I25+I30</f>
+        <v>3.2786885245901636</v>
       </c>
       <c r="J32" s="61">
-        <f>J56</f>
-        <v>112666.20846875</v>
+        <f ca="1">J56</f>
+        <v>112666.20846875013</v>
       </c>
       <c r="K32" s="62">
-        <f>IFERROR(I32/I$32,0)</f>
+        <f ca="1">IFERROR(I32/I$32,0)</f>
         <v>1</v>
       </c>
       <c r="L32" s="25"/>
@@ -4318,7 +4256,7 @@
       <c r="G34" s="62"/>
       <c r="H34" s="77"/>
       <c r="I34" s="76">
-        <f>IFERROR(I25/J11,0)</f>
+        <f ca="1">IFERROR(I25/J11,0)</f>
         <v>0</v>
       </c>
       <c r="J34" s="62"/>
@@ -4408,8 +4346,8 @@
       <c r="G36" s="62"/>
       <c r="H36" s="25"/>
       <c r="I36" s="76">
-        <f>IFERROR(I32/J6,0)</f>
-        <v>4.1502386387217302E-2</v>
+        <f ca="1">IFERROR(I32/J6,0)</f>
+        <v>4.150238638721726E-2</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="62"/>
@@ -4453,7 +4391,7 @@
       <c r="G37" s="79"/>
       <c r="H37" s="25"/>
       <c r="I37" s="78">
-        <f>IFERROR(1-(I24+I29)/I32,0)</f>
+        <f ca="1">IFERROR(1-(I24+I29)/I32,0)</f>
         <v>1</v>
       </c>
       <c r="J37" s="79"/>
@@ -4921,8 +4859,8 @@
         <v>2207364.5857923501</v>
       </c>
       <c r="J47" s="53">
-        <f>IFERROR((I47/I23)/12,0)</f>
-        <v>56103.849888888901</v>
+        <f ca="1">IFERROR((I47/I23)/12,0)</f>
+        <v>56103.849888888908</v>
       </c>
       <c r="K47" s="54">
         <f>IFERROR(I47/I$68,0)</f>
@@ -5061,8 +4999,8 @@
         <v>2207364.5857923501</v>
       </c>
       <c r="J49" s="110">
-        <f>IFERROR((I49/I25)/12,0)</f>
-        <v>56103.849888888901</v>
+        <f ca="1">IFERROR((I49/I25)/12,0)</f>
+        <v>56103.849888888908</v>
       </c>
       <c r="K49" s="111">
         <f>IFERROR(I49/I$68,0)</f>
@@ -5370,8 +5308,8 @@
         <v>-7247.7232240437197</v>
       </c>
       <c r="J54" s="53">
-        <f>IFERROR((I54/I32)/12,0)</f>
-        <v>-184.21296527777801</v>
+        <f ca="1">IFERROR((I54/I32)/12,0)</f>
+        <v>-184.2129652777779</v>
       </c>
       <c r="K54" s="54">
         <f t="shared" si="1"/>
@@ -5440,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="53">
-        <f>IFERROR((I55/I32)/12,0)</f>
+        <f ca="1">IFERROR((I55/I32)/12,0)</f>
         <v>0</v>
       </c>
       <c r="K55" s="54">
@@ -5508,8 +5446,8 @@
         <v>4432768.8577868901</v>
       </c>
       <c r="J56" s="61">
-        <f>IFERROR((I56/I32)/12,0)</f>
-        <v>112666.20846875</v>
+        <f ca="1">IFERROR((I56/I32)/12,0)</f>
+        <v>112666.20846875013</v>
       </c>
       <c r="K56" s="62">
         <f t="shared" si="1"/>
@@ -5640,8 +5578,8 @@
         <v>883813.73251366103</v>
       </c>
       <c r="J59" s="53">
-        <f>IFERROR((I$59/I$25)/12,0)</f>
-        <v>22463.5990347222</v>
+        <f ca="1">IFERROR((I$59/I$25)/12,0)</f>
+        <v>22463.599034722221</v>
       </c>
       <c r="K59" s="54">
         <f>IFERROR(I59/I$68,0)</f>
@@ -5780,7 +5718,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="53">
-        <f>IFERROR((I$61/I$32)/12,0)</f>
+        <f ca="1">IFERROR((I$61/I$32)/12,0)</f>
         <v>0</v>
       </c>
       <c r="K61" s="54">
@@ -5850,7 +5788,7 @@
         <v>5684.4262295081999</v>
       </c>
       <c r="J62" s="53">
-        <f>IFERROR((I$61/I$32)/12,0)</f>
+        <f ca="1">IFERROR((I$61/I$32)/12,0)</f>
         <v>0</v>
       </c>
       <c r="K62" s="54">
@@ -5916,8 +5854,8 @@
         <v>2200555.5606557401</v>
       </c>
       <c r="J63" s="61">
-        <f>IFERROR((I$63/I$32)/12,0)</f>
-        <v>55930.787166666698</v>
+        <f ca="1">IFERROR((I$63/I$32)/12,0)</f>
+        <v>55930.787166666734</v>
       </c>
       <c r="K63" s="62">
         <f>IFERROR(I63/I$68,0)</f>
@@ -6012,8 +5950,8 @@
         <v>267467.21311475401</v>
       </c>
       <c r="J65" s="53">
-        <f>IFERROR((I$65/I$32)/12,0)</f>
-        <v>6798.125</v>
+        <f ca="1">IFERROR((I$65/I$32)/12,0)</f>
+        <v>6798.1249999999991</v>
       </c>
       <c r="K65" s="54">
         <f>IFERROR(I65/I$68,0)</f>
@@ -6080,8 +6018,8 @@
         <v>-2889.6431693989098</v>
       </c>
       <c r="J66" s="53">
-        <f>IFERROR((I$66/I$32)/12,0)</f>
-        <v>-73.445097222222202</v>
+        <f ca="1">IFERROR((I$66/I$32)/12,0)</f>
+        <v>-73.445097222222302</v>
       </c>
       <c r="K66" s="54">
         <f>IFERROR(I66/I$68,0)</f>
@@ -6214,8 +6152,8 @@
         <v>6897901.9883879796</v>
       </c>
       <c r="J68" s="142">
-        <f>IFERROR(I68/(I$32*I$96*I$95),0)</f>
-        <v>175802.00889583299</v>
+        <f ca="1">IFERROR(I68/(I$32*I$96*I$95),0)</f>
+        <v>175802.00889583331</v>
       </c>
       <c r="K68" s="143">
         <f>IFERROR(I68/I$68,0)</f>
@@ -6415,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="45">
-        <f t="shared" ref="J72:J87" si="6">IFERROR((I72/I$32)/12,0)</f>
+        <f t="shared" ref="J72:J87" ca="1" si="6">IFERROR((I72/I$32)/12,0)</f>
         <v>0</v>
       </c>
       <c r="K72" s="46">
@@ -6484,8 +6422,8 @@
         <v>721852.75122950797</v>
       </c>
       <c r="J73" s="53">
-        <f t="shared" si="6"/>
-        <v>18347.090760416701</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>18347.09076041666</v>
       </c>
       <c r="K73" s="54">
         <f t="shared" si="7"/>
@@ -6554,8 +6492,8 @@
         <v>259432.80519125701</v>
       </c>
       <c r="J74" s="53">
-        <f t="shared" si="6"/>
-        <v>6593.9171319444404</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6593.9171319444495</v>
       </c>
       <c r="K74" s="54">
         <f t="shared" si="7"/>
@@ -6624,8 +6562,8 @@
         <v>167878.66844262299</v>
       </c>
       <c r="J75" s="53">
-        <f t="shared" si="6"/>
-        <v>4266.9161562500003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>4266.9161562500012</v>
       </c>
       <c r="K75" s="54">
         <f t="shared" si="7"/>
@@ -6694,7 +6632,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="53">
-        <f t="shared" si="6"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
       <c r="K76" s="54">
@@ -6764,8 +6702,8 @@
         <v>832809.988797814</v>
       </c>
       <c r="J77" s="53">
-        <f t="shared" si="6"/>
-        <v>21167.253881944402</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>21167.253881944442</v>
       </c>
       <c r="K77" s="54">
         <f t="shared" si="7"/>
@@ -6834,8 +6772,8 @@
         <v>417218.67513661197</v>
       </c>
       <c r="J78" s="53">
-        <f t="shared" si="6"/>
-        <v>10604.3079930556</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>10604.307993055556</v>
       </c>
       <c r="K78" s="54">
         <f t="shared" si="7"/>
@@ -6904,8 +6842,8 @@
         <v>1400820.08674863</v>
       </c>
       <c r="J79" s="53">
-        <f t="shared" si="6"/>
-        <v>35604.177204861102</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>35604.177204861022</v>
       </c>
       <c r="K79" s="54">
         <f t="shared" si="7"/>
@@ -6974,8 +6912,8 @@
         <v>1562941.4087431701</v>
       </c>
       <c r="J80" s="53">
-        <f t="shared" si="6"/>
-        <v>39724.760805555597</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>39724.760805555576</v>
       </c>
       <c r="K80" s="54">
         <f t="shared" si="7"/>
@@ -7044,8 +6982,8 @@
         <v>4724.0972677595601</v>
       </c>
       <c r="J81" s="53">
-        <f t="shared" si="6"/>
-        <v>120.07080555555601</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>120.07080555555551</v>
       </c>
       <c r="K81" s="54">
         <f t="shared" si="7"/>
@@ -7114,8 +7052,8 @@
         <v>238503.17663934399</v>
       </c>
       <c r="J82" s="53">
-        <f t="shared" si="6"/>
-        <v>6061.9557395833299</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6061.9557395833262</v>
       </c>
       <c r="K82" s="54">
         <f t="shared" si="7"/>
@@ -7184,8 +7122,8 @@
         <v>59725.737841530099</v>
       </c>
       <c r="J83" s="53">
-        <f t="shared" si="6"/>
-        <v>1518.0291701388901</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1518.0291701388903</v>
       </c>
       <c r="K83" s="54">
         <f t="shared" si="7"/>
@@ -7254,8 +7192,8 @@
         <v>209611.02322404401</v>
       </c>
       <c r="J84" s="53">
-        <f t="shared" si="6"/>
-        <v>5327.6135069444399</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5327.6135069444526</v>
       </c>
       <c r="K84" s="54">
         <f t="shared" si="7"/>
@@ -7324,8 +7262,8 @@
         <v>273313.78510928998</v>
       </c>
       <c r="J85" s="53">
-        <f t="shared" si="6"/>
-        <v>6946.7253715277802</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6946.7253715277875</v>
       </c>
       <c r="K85" s="54">
         <f t="shared" si="7"/>
@@ -7394,8 +7332,8 @@
         <v>20234.114071038301</v>
       </c>
       <c r="J86" s="53">
-        <f t="shared" si="6"/>
-        <v>514.28373263888898</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>514.28373263889023</v>
       </c>
       <c r="K86" s="54">
         <f t="shared" si="7"/>
@@ -7464,8 +7402,8 @@
         <v>426582.50081967202</v>
       </c>
       <c r="J87" s="161">
-        <f t="shared" si="6"/>
-        <v>10842.305229166701</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>10842.305229166665</v>
       </c>
       <c r="K87" s="135">
         <f t="shared" si="7"/>
@@ -7532,8 +7470,8 @@
         <v>6169066.3184426203</v>
       </c>
       <c r="J88" s="142">
-        <f>IFERROR(I88/(I$32*I$96*I$95),0)</f>
-        <v>157226.68336250001</v>
+        <f ca="1">IFERROR(I88/(I$32*I$96*I$95),0)</f>
+        <v>157226.6833624999</v>
       </c>
       <c r="K88" s="143">
         <f t="shared" si="7"/>
@@ -7626,8 +7564,8 @@
         <v>728835.66994535597</v>
       </c>
       <c r="J90" s="142">
-        <f>IFERROR(I90/(I$32*I$96*I$95),0)</f>
-        <v>18575.3255333333</v>
+        <f ca="1">IFERROR(I90/(I$32*I$96*I$95),0)</f>
+        <v>18575.325533333347</v>
       </c>
       <c r="K90" s="143">
         <f>IFERROR(I90/I$68,0)</f>
@@ -7693,8 +7631,8 @@
         <v>344895.09941939899</v>
       </c>
       <c r="J91" s="53">
-        <f>IFERROR((I91/$I$32)/12,0)</f>
-        <v>8766.0837769097197</v>
+        <f ca="1">IFERROR((I91/$I$32)/12,0)</f>
+        <v>8766.0837769097252</v>
       </c>
       <c r="K91" s="54">
         <f>IFERROR(I91/I$68,0)</f>
@@ -7758,8 +7696,8 @@
         <v>383940.57052595698</v>
       </c>
       <c r="J92" s="142">
-        <f>IFERROR(I92/(I$32*I$96*I$95),0)</f>
-        <v>9785.2250885416706</v>
+        <f ca="1">IFERROR(I92/(I$32*I$96*I$95),0)</f>
+        <v>9785.2250885416815</v>
       </c>
       <c r="K92" s="143">
         <f>IFERROR(I92/I$68,0)</f>
@@ -8606,7 +8544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="5:23" ht="18.75" hidden="1" customHeight="1">
+    <row r="113" spans="1:23" ht="18.75" hidden="1" customHeight="1">
       <c r="E113" s="201" t="s">
         <v>115</v>
       </c>
@@ -8641,7 +8579,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="5:23" ht="18.75" hidden="1" customHeight="1">
+    <row r="114" spans="1:23" ht="18.75" hidden="1" customHeight="1">
       <c r="E114" s="203">
         <f>E88+E87</f>
         <v>3879325.78</v>
@@ -8671,7 +8609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="5:23" ht="18.75" hidden="1" customHeight="1">
+    <row r="115" spans="1:23" ht="18.75" hidden="1" customHeight="1">
       <c r="E115" s="208"/>
       <c r="F115" s="209" t="s">
         <v>114</v>
@@ -8702,6 +8640,90 @@
         <f>IFERROR(W114/U114,0)</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="124" spans="1:23" ht="18.75" customHeight="1">
+      <c r="A124" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" ht="18.75" customHeight="1">
+      <c r="A125" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B125" s="18">
+        <f>N6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" ht="18.75" customHeight="1">
+      <c r="A126" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" ht="18.75" customHeight="1">
+      <c r="A127" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" ht="18.75" customHeight="1">
+      <c r="A128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+    </row>
+    <row r="130" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A130" s="12"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="12"/>
+    </row>
+    <row r="131" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A131" s="12" t="str">
+        <f>"'"&amp;$A125&amp;"'"&amp;"!"&amp;A127</f>
+        <v>'Asset Codes'!$H$1:$BZ$1</v>
+      </c>
+      <c r="B131" s="12" t="str">
+        <f>"'"&amp;$A125&amp;"'"&amp;"!"&amp;B127</f>
+        <v>'Asset Codes'!$B$2:$B$500</v>
+      </c>
+      <c r="C131" s="12" t="str">
+        <f>"'"&amp;$A125&amp;"'"&amp;"!"&amp;C127</f>
+        <v>'Asset Codes'!$H$2:$BZ$500</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A132" s="32"/>
+      <c r="B132" s="32"/>
+      <c r="C132" s="32"/>
+    </row>
+    <row r="133" spans="1:11" ht="18.75" customHeight="1">
+      <c r="I133" s="32"/>
+      <c r="J133" s="32"/>
+      <c r="K133" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G112 K112 O112 S112 W112 G115 K115 O115 S115 W115">
@@ -8739,32 +8761,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B3" s="259" t="s">
+      <c r="B3" s="276" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="259"/>
-      <c r="D3" s="259"/>
-      <c r="E3" s="259"/>
-      <c r="F3" s="259"/>
-      <c r="G3" s="259"/>
-      <c r="H3" s="259"/>
-      <c r="I3" s="259"/>
-      <c r="J3" s="259"/>
-      <c r="L3" s="260" t="s">
+      <c r="C3" s="276"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="276"/>
+      <c r="F3" s="276"/>
+      <c r="G3" s="276"/>
+      <c r="H3" s="276"/>
+      <c r="I3" s="276"/>
+      <c r="J3" s="276"/>
+      <c r="L3" s="277" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="260"/>
+      <c r="M3" s="277"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" customHeight="1">
-      <c r="B4" s="259"/>
-      <c r="C4" s="259"/>
-      <c r="D4" s="259"/>
-      <c r="E4" s="259"/>
-      <c r="F4" s="259"/>
-      <c r="G4" s="259"/>
-      <c r="H4" s="259"/>
-      <c r="I4" s="259"/>
-      <c r="J4" s="259"/>
+      <c r="B4" s="276"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="276"/>
+      <c r="J4" s="276"/>
       <c r="L4" s="177" t="s">
         <v>97</v>
       </c>
@@ -8775,14 +8797,14 @@
     </row>
     <row r="5" spans="2:13" ht="21" customHeight="1">
       <c r="B5" s="211"/>
-      <c r="C5" s="261" t="s">
+      <c r="C5" s="278" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261" t="s">
+      <c r="D5" s="278"/>
+      <c r="E5" s="278" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="261"/>
+      <c r="F5" s="278"/>
       <c r="G5" s="212"/>
       <c r="H5" s="212"/>
       <c r="I5" s="212"/>
@@ -8797,516 +8819,516 @@
     </row>
     <row r="6" spans="2:13" ht="18.75" customHeight="1">
       <c r="B6" s="214"/>
-      <c r="C6" s="262" t="s">
+      <c r="C6" s="279" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="262"/>
-      <c r="E6" s="262" t="s">
+      <c r="D6" s="279"/>
+      <c r="E6" s="279" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="262"/>
-      <c r="G6" s="263" t="s">
+      <c r="F6" s="279"/>
+      <c r="G6" s="280" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="263"/>
-      <c r="I6" s="264" t="s">
+      <c r="H6" s="280"/>
+      <c r="I6" s="281" t="s">
         <v>124</v>
       </c>
-      <c r="J6" s="264"/>
+      <c r="J6" s="281"/>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1">
       <c r="B7" s="215" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="265"/>
-      <c r="D7" s="265"/>
-      <c r="E7" s="265"/>
-      <c r="F7" s="265"/>
-      <c r="G7" s="265"/>
-      <c r="H7" s="265"/>
-      <c r="I7" s="266"/>
-      <c r="J7" s="266"/>
+      <c r="C7" s="269"/>
+      <c r="D7" s="269"/>
+      <c r="E7" s="269"/>
+      <c r="F7" s="269"/>
+      <c r="G7" s="269"/>
+      <c r="H7" s="269"/>
+      <c r="I7" s="271"/>
+      <c r="J7" s="271"/>
     </row>
     <row r="8" spans="2:13" ht="18.75" customHeight="1">
       <c r="B8" s="216" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="267"/>
-      <c r="D8" s="267"/>
-      <c r="E8" s="268">
+      <c r="C8" s="275"/>
+      <c r="D8" s="275"/>
+      <c r="E8" s="270">
         <f>'Detailed Model'!M32</f>
         <v>0</v>
       </c>
-      <c r="F8" s="268"/>
-      <c r="G8" s="269">
+      <c r="F8" s="270"/>
+      <c r="G8" s="266">
         <f>IFERROR((E8-C8)/C8,0)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="269"/>
-      <c r="I8" s="266">
+      <c r="H8" s="266"/>
+      <c r="I8" s="271">
         <f t="shared" ref="I8:I16" si="0">E8-C8</f>
         <v>0</v>
       </c>
-      <c r="J8" s="266"/>
+      <c r="J8" s="271"/>
     </row>
     <row r="9" spans="2:13" ht="18.75" customHeight="1">
       <c r="B9" s="216" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="269"/>
-      <c r="D9" s="269"/>
-      <c r="E9" s="269">
+      <c r="C9" s="266"/>
+      <c r="D9" s="266"/>
+      <c r="E9" s="266">
         <f>'Detailed Model'!M36</f>
         <v>0</v>
       </c>
-      <c r="F9" s="269"/>
-      <c r="G9" s="269">
+      <c r="F9" s="266"/>
+      <c r="G9" s="266">
         <f>IFERROR(((E9*100)-(C9*100))/(C9*100),0)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="269"/>
-      <c r="I9" s="270">
+      <c r="H9" s="266"/>
+      <c r="I9" s="272">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="270"/>
+      <c r="J9" s="272"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" customHeight="1">
       <c r="B10" s="216" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="271"/>
-      <c r="D10" s="271"/>
-      <c r="E10" s="271">
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265">
         <f>'Detailed Model'!M68</f>
         <v>0</v>
       </c>
-      <c r="F10" s="271"/>
-      <c r="G10" s="269">
+      <c r="F10" s="265"/>
+      <c r="G10" s="266">
         <f t="shared" ref="G10:G16" si="1">IFERROR((E10-C10)/C10,0)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="269"/>
-      <c r="I10" s="272">
+      <c r="H10" s="266"/>
+      <c r="I10" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="272"/>
+      <c r="J10" s="267"/>
     </row>
     <row r="11" spans="2:13" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B11" s="217" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="271"/>
-      <c r="D11" s="271"/>
-      <c r="E11" s="271">
+      <c r="C11" s="265"/>
+      <c r="D11" s="265"/>
+      <c r="E11" s="265">
         <f>'Detailed Model'!N47</f>
         <v>0</v>
       </c>
-      <c r="F11" s="271"/>
-      <c r="G11" s="269">
+      <c r="F11" s="265"/>
+      <c r="G11" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="269"/>
-      <c r="I11" s="272">
+      <c r="H11" s="266"/>
+      <c r="I11" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="272"/>
+      <c r="J11" s="267"/>
     </row>
     <row r="12" spans="2:13" ht="18.75" customHeight="1">
       <c r="B12" s="216" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="271"/>
-      <c r="D12" s="271"/>
-      <c r="E12" s="271">
+      <c r="C12" s="265"/>
+      <c r="D12" s="265"/>
+      <c r="E12" s="265">
         <f>'Detailed Model'!M88+'Detailed Model'!M91</f>
         <v>0</v>
       </c>
-      <c r="F12" s="271"/>
-      <c r="G12" s="269">
+      <c r="F12" s="265"/>
+      <c r="G12" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="269"/>
-      <c r="I12" s="272">
+      <c r="H12" s="266"/>
+      <c r="I12" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="272"/>
+      <c r="J12" s="267"/>
     </row>
     <row r="13" spans="2:13" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B13" s="217" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="271"/>
-      <c r="D13" s="271"/>
-      <c r="E13" s="271">
+      <c r="C13" s="265"/>
+      <c r="D13" s="265"/>
+      <c r="E13" s="265">
         <f>'Detailed Model'!M72</f>
         <v>0</v>
       </c>
-      <c r="F13" s="271"/>
-      <c r="G13" s="269">
+      <c r="F13" s="265"/>
+      <c r="G13" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="269"/>
-      <c r="I13" s="272">
+      <c r="H13" s="266"/>
+      <c r="I13" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="272"/>
+      <c r="J13" s="267"/>
     </row>
     <row r="14" spans="2:13" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B14" s="217" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="271"/>
-      <c r="D14" s="271"/>
-      <c r="E14" s="271">
+      <c r="C14" s="265"/>
+      <c r="D14" s="265"/>
+      <c r="E14" s="265">
         <f>'Detailed Model'!M73</f>
         <v>0</v>
       </c>
-      <c r="F14" s="271"/>
-      <c r="G14" s="269">
+      <c r="F14" s="265"/>
+      <c r="G14" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="269"/>
-      <c r="I14" s="272">
+      <c r="H14" s="266"/>
+      <c r="I14" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="272"/>
+      <c r="J14" s="267"/>
     </row>
     <row r="15" spans="2:13" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B15" s="217" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="271"/>
-      <c r="D15" s="271"/>
-      <c r="E15" s="271">
+      <c r="C15" s="265"/>
+      <c r="D15" s="265"/>
+      <c r="E15" s="265">
         <f>'Detailed Model'!M77</f>
         <v>0</v>
       </c>
-      <c r="F15" s="271"/>
-      <c r="G15" s="269">
+      <c r="F15" s="265"/>
+      <c r="G15" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="269"/>
-      <c r="I15" s="272">
+      <c r="H15" s="266"/>
+      <c r="I15" s="267">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="272"/>
+      <c r="J15" s="267"/>
     </row>
     <row r="16" spans="2:13" ht="18.75" customHeight="1">
       <c r="B16" s="218" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="271">
+      <c r="C16" s="265">
         <f>C10-C12</f>
         <v>0</v>
       </c>
-      <c r="D16" s="271"/>
-      <c r="E16" s="271">
+      <c r="D16" s="265"/>
+      <c r="E16" s="265">
         <f>E10-E12</f>
         <v>0</v>
       </c>
-      <c r="F16" s="271"/>
-      <c r="G16" s="269">
+      <c r="F16" s="265"/>
+      <c r="G16" s="266">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="269"/>
-      <c r="I16" s="273">
+      <c r="H16" s="266"/>
+      <c r="I16" s="268">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="273"/>
+      <c r="J16" s="268"/>
     </row>
     <row r="17" spans="2:10" ht="18.75" customHeight="1">
       <c r="B17" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="274">
+      <c r="C17" s="259">
         <f>IFERROR((C16/C10),0)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="274"/>
-      <c r="E17" s="274">
+      <c r="D17" s="259"/>
+      <c r="E17" s="259">
         <f>IFERROR((E16/E10),0)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="274"/>
-      <c r="G17" s="275"/>
-      <c r="H17" s="275"/>
-      <c r="I17" s="276">
+      <c r="F17" s="259"/>
+      <c r="G17" s="273"/>
+      <c r="H17" s="273"/>
+      <c r="I17" s="261">
         <f>IFERROR((E17-C17),0)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="276"/>
+      <c r="J17" s="261"/>
     </row>
     <row r="18" spans="2:10" ht="18.75" customHeight="1">
       <c r="B18" s="214"/>
-      <c r="C18" s="265"/>
-      <c r="D18" s="265"/>
-      <c r="E18" s="265"/>
-      <c r="F18" s="265"/>
-      <c r="G18" s="265"/>
-      <c r="H18" s="265"/>
-      <c r="I18" s="277"/>
-      <c r="J18" s="277"/>
+      <c r="C18" s="269"/>
+      <c r="D18" s="269"/>
+      <c r="E18" s="269"/>
+      <c r="F18" s="269"/>
+      <c r="G18" s="269"/>
+      <c r="H18" s="269"/>
+      <c r="I18" s="274"/>
+      <c r="J18" s="274"/>
     </row>
     <row r="19" spans="2:10" ht="18.75" customHeight="1">
       <c r="B19" s="215" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="265"/>
-      <c r="D19" s="265"/>
-      <c r="E19" s="265"/>
-      <c r="F19" s="265"/>
-      <c r="G19" s="265"/>
-      <c r="H19" s="265"/>
-      <c r="I19" s="277"/>
-      <c r="J19" s="277"/>
+      <c r="C19" s="269"/>
+      <c r="D19" s="269"/>
+      <c r="E19" s="269"/>
+      <c r="F19" s="269"/>
+      <c r="G19" s="269"/>
+      <c r="H19" s="269"/>
+      <c r="I19" s="274"/>
+      <c r="J19" s="274"/>
     </row>
     <row r="20" spans="2:10" ht="18.75" customHeight="1">
       <c r="B20" s="216" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="265"/>
-      <c r="D20" s="265"/>
-      <c r="E20" s="268">
+      <c r="C20" s="269"/>
+      <c r="D20" s="269"/>
+      <c r="E20" s="270">
         <f>'Detailed Model'!Q32</f>
         <v>0</v>
       </c>
-      <c r="F20" s="268"/>
-      <c r="G20" s="269">
+      <c r="F20" s="270"/>
+      <c r="G20" s="266">
         <f>IFERROR((E20-C20)/C20,0)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="269"/>
-      <c r="I20" s="266">
+      <c r="H20" s="266"/>
+      <c r="I20" s="271">
         <f t="shared" ref="I20:I28" si="2">E20-C20</f>
         <v>0</v>
       </c>
-      <c r="J20" s="266"/>
+      <c r="J20" s="271"/>
     </row>
     <row r="21" spans="2:10" ht="18.75" customHeight="1">
       <c r="B21" s="216" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="269"/>
-      <c r="D21" s="269"/>
-      <c r="E21" s="269">
+      <c r="C21" s="266"/>
+      <c r="D21" s="266"/>
+      <c r="E21" s="266">
         <f>'Detailed Model'!Q36</f>
         <v>0</v>
       </c>
-      <c r="F21" s="269"/>
-      <c r="G21" s="269">
+      <c r="F21" s="266"/>
+      <c r="G21" s="266">
         <f>IFERROR(((E21*100)-(C21*100))/(C21*100),0)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="269"/>
-      <c r="I21" s="270">
+      <c r="H21" s="266"/>
+      <c r="I21" s="272">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J21" s="270"/>
+      <c r="J21" s="272"/>
     </row>
     <row r="22" spans="2:10" ht="18.75" customHeight="1">
       <c r="B22" s="216" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="271"/>
-      <c r="D22" s="271"/>
-      <c r="E22" s="271">
+      <c r="C22" s="265"/>
+      <c r="D22" s="265"/>
+      <c r="E22" s="265">
         <f>'Detailed Model'!Q68</f>
         <v>0</v>
       </c>
-      <c r="F22" s="271"/>
-      <c r="G22" s="269">
+      <c r="F22" s="265"/>
+      <c r="G22" s="266">
         <f t="shared" ref="G22:G28" si="3">IFERROR((E22-C22)/C22,0)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="269"/>
-      <c r="I22" s="272">
+      <c r="H22" s="266"/>
+      <c r="I22" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="272"/>
+      <c r="J22" s="267"/>
     </row>
     <row r="23" spans="2:10" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B23" s="217" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="271"/>
-      <c r="D23" s="271"/>
-      <c r="E23" s="271">
+      <c r="C23" s="265"/>
+      <c r="D23" s="265"/>
+      <c r="E23" s="265">
         <f>'Detailed Model'!R47</f>
         <v>0</v>
       </c>
-      <c r="F23" s="271"/>
-      <c r="G23" s="269">
+      <c r="F23" s="265"/>
+      <c r="G23" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H23" s="269"/>
-      <c r="I23" s="272">
+      <c r="H23" s="266"/>
+      <c r="I23" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="272"/>
+      <c r="J23" s="267"/>
     </row>
     <row r="24" spans="2:10" ht="18.75" customHeight="1">
       <c r="B24" s="216" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="271"/>
-      <c r="D24" s="271"/>
-      <c r="E24" s="271">
+      <c r="C24" s="265"/>
+      <c r="D24" s="265"/>
+      <c r="E24" s="265">
         <f>'Detailed Model'!Q88+'Detailed Model'!Q91</f>
         <v>0</v>
       </c>
-      <c r="F24" s="271"/>
-      <c r="G24" s="269">
+      <c r="F24" s="265"/>
+      <c r="G24" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H24" s="269"/>
-      <c r="I24" s="272">
+      <c r="H24" s="266"/>
+      <c r="I24" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="272"/>
+      <c r="J24" s="267"/>
     </row>
     <row r="25" spans="2:10" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B25" s="217" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="271"/>
-      <c r="D25" s="271"/>
-      <c r="E25" s="271">
+      <c r="C25" s="265"/>
+      <c r="D25" s="265"/>
+      <c r="E25" s="265">
         <f>'Detailed Model'!Q72</f>
         <v>0</v>
       </c>
-      <c r="F25" s="271"/>
-      <c r="G25" s="269">
+      <c r="F25" s="265"/>
+      <c r="G25" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H25" s="269"/>
-      <c r="I25" s="272">
+      <c r="H25" s="266"/>
+      <c r="I25" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="272"/>
+      <c r="J25" s="267"/>
     </row>
     <row r="26" spans="2:10" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B26" s="217" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="271"/>
-      <c r="D26" s="271"/>
-      <c r="E26" s="271">
+      <c r="C26" s="265"/>
+      <c r="D26" s="265"/>
+      <c r="E26" s="265">
         <f>'Detailed Model'!Q73</f>
         <v>0</v>
       </c>
-      <c r="F26" s="271"/>
-      <c r="G26" s="269">
+      <c r="F26" s="265"/>
+      <c r="G26" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H26" s="269"/>
-      <c r="I26" s="272">
+      <c r="H26" s="266"/>
+      <c r="I26" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="272"/>
+      <c r="J26" s="267"/>
     </row>
     <row r="27" spans="2:10" ht="18.75" customHeight="1" outlineLevel="1" collapsed="1">
       <c r="B27" s="217" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="271"/>
-      <c r="D27" s="271"/>
-      <c r="E27" s="271">
+      <c r="C27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="265">
         <f>'Detailed Model'!Q77</f>
         <v>0</v>
       </c>
-      <c r="F27" s="271"/>
-      <c r="G27" s="269">
+      <c r="F27" s="265"/>
+      <c r="G27" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H27" s="269"/>
-      <c r="I27" s="272">
+      <c r="H27" s="266"/>
+      <c r="I27" s="267">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="272"/>
+      <c r="J27" s="267"/>
     </row>
     <row r="28" spans="2:10" ht="18.75" customHeight="1">
       <c r="B28" s="218" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="271">
+      <c r="C28" s="265">
         <f>C22-C24</f>
         <v>0</v>
       </c>
-      <c r="D28" s="271"/>
-      <c r="E28" s="271">
+      <c r="D28" s="265"/>
+      <c r="E28" s="265">
         <f>E22-E24</f>
         <v>0</v>
       </c>
-      <c r="F28" s="271"/>
-      <c r="G28" s="269">
+      <c r="F28" s="265"/>
+      <c r="G28" s="266">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="269"/>
-      <c r="I28" s="273">
+      <c r="H28" s="266"/>
+      <c r="I28" s="268">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="273"/>
+      <c r="J28" s="268"/>
     </row>
     <row r="29" spans="2:10" ht="18.75" customHeight="1">
       <c r="B29" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="274">
+      <c r="C29" s="259">
         <f>IFERROR((C28/C22),0)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="274"/>
-      <c r="E29" s="274">
+      <c r="D29" s="259"/>
+      <c r="E29" s="259">
         <f>IFERROR((E28/E22),0)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="274"/>
-      <c r="G29" s="278"/>
-      <c r="H29" s="278"/>
-      <c r="I29" s="276">
+      <c r="F29" s="259"/>
+      <c r="G29" s="260"/>
+      <c r="H29" s="260"/>
+      <c r="I29" s="261">
         <f>IFERROR((E29-C29),0)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="276"/>
+      <c r="J29" s="261"/>
     </row>
     <row r="30" spans="2:10" ht="18.75" customHeight="1">
       <c r="B30" s="220"/>
-      <c r="C30" s="279"/>
-      <c r="D30" s="279"/>
-      <c r="E30" s="279"/>
-      <c r="F30" s="279"/>
-      <c r="G30" s="280"/>
-      <c r="H30" s="280"/>
-      <c r="I30" s="281"/>
-      <c r="J30" s="281"/>
+      <c r="C30" s="262"/>
+      <c r="D30" s="262"/>
+      <c r="E30" s="262"/>
+      <c r="F30" s="262"/>
+      <c r="G30" s="263"/>
+      <c r="H30" s="263"/>
+      <c r="I30" s="264"/>
+      <c r="J30" s="264"/>
     </row>
     <row r="31" spans="2:10" ht="18.75" customHeight="1">
       <c r="B31" s="223"/>
@@ -9391,6 +9413,90 @@
     </row>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="G29:H29"/>
@@ -9411,90 +9517,6 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>